<commit_message>
Return button from entity page, buttons on bottom, states translated, sorting started
</commit_message>
<xml_diff>
--- a/requirements/BugTracking.xlsx
+++ b/requirements/BugTracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Gena\Local\Work\_Drive\Projects\Verum\EasyBudget\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikita\Git\EasyBudget\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCCA784-FD54-4036-8498-020C0A81E480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF38E758-EE7A-4861-A60B-D234E5A19C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{07F58553-A4A0-4277-86D4-14AF11B81E43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07F58553-A4A0-4277-86D4-14AF11B81E43}"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="25">
   <si>
     <t>Bug</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Add info panel (probably on the top)</t>
+  </si>
+  <si>
+    <t>Localization file added in common</t>
+  </si>
+  <si>
+    <t>Added button at the bottom of entity page</t>
   </si>
 </sst>
 </file>
@@ -456,7 +462,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,13 +502,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="1">
         <v>44158</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -513,7 +522,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -530,7 +539,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -581,13 +590,16 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="1">
         <v>44158</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sorting finished, icons added
</commit_message>
<xml_diff>
--- a/requirements/BugTracking.xlsx
+++ b/requirements/BugTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikita\Git\EasyBudget\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF38E758-EE7A-4861-A60B-D234E5A19C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4437672D-5CB3-4927-9067-336D6E406EC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07F58553-A4A0-4277-86D4-14AF11B81E43}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -573,7 +573,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -644,7 +644,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Postpone and Reject buttons added
</commit_message>
<xml_diff>
--- a/requirements/BugTracking.xlsx
+++ b/requirements/BugTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikita\Git\EasyBudget\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5757A0D1-C180-4EF6-88DB-141241D73CF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250FD4E0-D4DF-4E8E-8C23-342B0DCBCCEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07F58553-A4A0-4277-86D4-14AF11B81E43}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +739,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -756,7 +756,7 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>

</xml_diff>